<commit_message>
Fix for unseen issue with default comment font.
</commit_message>
<xml_diff>
--- a/test/perl_output/comments2.xlsx
+++ b/test/perl_output/comments2.xlsx
@@ -523,9 +523,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -833,12 +832,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:3" ht="50" customHeight="1">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="3:3" ht="50" customHeight="1">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -860,12 +859,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:3" ht="50" customHeight="1">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="3:3" ht="50" customHeight="1">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -887,17 +886,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:3" ht="50" customHeight="1">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="3:3" ht="50" customHeight="1">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="3:3" ht="50" customHeight="1">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -919,27 +918,27 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:3" ht="50" customHeight="1">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="3:3" ht="50" customHeight="1">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="3:3" ht="50" customHeight="1">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="3:3" ht="50" customHeight="1">
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="3:3">
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -961,22 +960,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:3" ht="50" customHeight="1">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="3:3" ht="50" customHeight="1">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="3:3" ht="50" customHeight="1">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="3:3" ht="50" customHeight="1">
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -998,17 +997,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:3" ht="50" customHeight="1">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="3:3" ht="50" customHeight="1">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="3:3" ht="50" customHeight="1">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1030,17 +1029,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:3" ht="50" customHeight="1">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="3:3" ht="50" customHeight="1">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="3:3" ht="50" customHeight="1">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1062,12 +1061,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:3" ht="80" customHeight="1">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="3:3">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>